<commit_message>
[feat] load excel file when message recieved
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suzuki1230/Documents/dev/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532F4ACB-552C-E741-9FE6-4260D7BD5F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAF4357-5B08-0A4F-87C5-A3DD86E79FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2120" windowWidth="28300" windowHeight="17440" xr2:uid="{E6CF2D20-2F92-5042-9111-C2CE0EBFDC64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>player1</t>
     <phoneticPr fontId="1"/>
@@ -52,6 +52,25 @@
   <si>
     <t>player4</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>局本場</t>
+    <rPh sb="0" eb="1">
+      <t>🎵</t>
+    </rPh>
+    <rPh sb="1" eb="3">
+      <t xml:space="preserve">ホンバ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>player2</t>
+  </si>
+  <si>
+    <t>player3</t>
+  </si>
+  <si>
+    <t>player4</t>
   </si>
 </sst>
 </file>
@@ -435,44 +454,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DFEBD9-B0F3-124C-920D-B401C71A8C28}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>30000</v>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9">
+      <c r="B2">
+        <v>8000</v>
+      </c>
+      <c r="C2">
+        <v>-8000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>25000+SUM(B:B)</f>
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3">
+        <v>-2000</v>
+      </c>
+      <c r="C3">
+        <v>-4000</v>
+      </c>
+      <c r="D3">
+        <v>8000</v>
+      </c>
+      <c r="E3">
+        <v>-2000</v>
+      </c>
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>40000</v>
+      <c r="I3">
+        <f>25000+SUM(C:C)</f>
+        <v>13000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:9">
+      <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>12000</v>
+      <c r="I4">
+        <f>25000+SUM(D:D)</f>
+        <v>33000</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9">
+      <c r="H5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>18000</v>
+      <c r="I5">
+        <f>25000+SUM(E:E)</f>
+        <v>23000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[feat] add keyword of messages
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suzuki1230/Documents/dev/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAF4357-5B08-0A4F-87C5-A3DD86E79FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67028E61-A984-E544-87E0-B0BEED91DEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2120" windowWidth="28300" windowHeight="17440" xr2:uid="{E6CF2D20-2F92-5042-9111-C2CE0EBFDC64}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="I2">
         <f>25000+SUM(B:B)</f>
-        <v>31000</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -512,16 +512,28 @@
       </c>
       <c r="I3">
         <f>25000+SUM(C:C)</f>
-        <v>13000</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="4" spans="1:9">
+      <c r="B4">
+        <v>-4000</v>
+      </c>
+      <c r="C4">
+        <v>8000</v>
+      </c>
+      <c r="D4">
+        <v>-2000</v>
+      </c>
+      <c r="E4">
+        <v>-2000</v>
+      </c>
       <c r="H4" t="s">
         <v>2</v>
       </c>
       <c r="I4">
         <f>25000+SUM(D:D)</f>
-        <v>33000</v>
+        <v>31000</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -530,7 +542,7 @@
       </c>
       <c r="I5">
         <f>25000+SUM(E:E)</f>
-        <v>23000</v>
+        <v>21000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[feat] add score result to excel file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,24 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suzuki1230/Documents/dev/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67028E61-A984-E544-87E0-B0BEED91DEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F8FF25-93D9-4546-AF26-5B592796111E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2120" windowWidth="28300" windowHeight="17440" xr2:uid="{E6CF2D20-2F92-5042-9111-C2CE0EBFDC64}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,32 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+  <si>
+    <t>局本場</t>
+  </si>
   <si>
     <t>player1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>player2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>player3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>player4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>局本場</t>
-    <rPh sb="0" eb="1">
-      <t>🎵</t>
-    </rPh>
-    <rPh sb="1" eb="3">
-      <t xml:space="preserve">ホンバ </t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>player2</t>
@@ -83,13 +60,12 @@
       <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
       <name val="游ゴシック"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -112,20 +88,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -453,100 +425,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DFEBD9-B0F3-124C-920D-B401C71A8C28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="B2">
-        <v>8000</v>
-      </c>
-      <c r="C2">
-        <v>-8000</v>
-      </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <f>25000+SUM(B:B)</f>
-        <v>27000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="B3">
-        <v>-2000</v>
-      </c>
-      <c r="C3">
-        <v>-4000</v>
-      </c>
-      <c r="D3">
-        <v>8000</v>
-      </c>
-      <c r="E3">
-        <v>-2000</v>
-      </c>
       <c r="H3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <f>25000+SUM(C:C)</f>
-        <v>21000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="B4">
-        <v>-4000</v>
-      </c>
-      <c r="C4">
-        <v>8000</v>
-      </c>
-      <c r="D4">
-        <v>-2000</v>
-      </c>
-      <c r="E4">
-        <v>-2000</v>
-      </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4">
         <f>25000+SUM(D:D)</f>
-        <v>31000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="H5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <f>25000+SUM(E:E)</f>
-        <v>21000</v>
+        <v>25000</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:I1 F2:I6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>